<commit_message>
Added test cases for Deffered,Autopay,Disabled Amount , Disabled Billing Address
</commit_message>
<xml_diff>
--- a/KatalonData/IWPBootstrapData/VRelayPaymentsCC.xlsx
+++ b/KatalonData/IWPBootstrapData/VRelayPaymentsCC.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T476640\Documents\VPS_Katalon\VPS-Katalon\KatalonData\IWPBootstrapData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{2E3B79ED-0D5B-4B27-BC03-A14D6E0D1350}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{676EBDAF-86A3-4BC1-A302-49CE2A5FE37D}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="2" windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{19E085DA-5ADF-4B16-9D78-B410FD3FCE3D}" yWindow="-110"/>
+    <workbookView activeTab="13" firstSheet="13" windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{19E085DA-5ADF-4B16-9D78-B410FD3FCE3D}" yWindow="-110"/>
   </bookViews>
   <sheets>
     <sheet name="PayNowCC" r:id="rId1" sheetId="1"/>
-    <sheet name="PayNowCreditCardSCF" r:id="rId2" sheetId="12"/>
-    <sheet name="PayNowCreditCardDCF" r:id="rId3" sheetId="13"/>
-    <sheet name="PayNowCCSCF" r:id="rId4" sheetId="5"/>
-    <sheet name="PayNowCCDCF" r:id="rId5" sheetId="6"/>
-    <sheet name="DCFVerbiage" r:id="rId6" sheetId="8"/>
-    <sheet name="OverUnderPay" r:id="rId7" sheetId="9"/>
-    <sheet name="MissingCC" r:id="rId8" sheetId="4"/>
-    <sheet name="Sheet2" r:id="rId9" sheetId="3"/>
-    <sheet name="NoModifyAmount" r:id="rId10" sheetId="10"/>
-    <sheet name="NoOverPay" r:id="rId11" sheetId="11"/>
-    <sheet name="SCFVerbiage" r:id="rId12" sheetId="7"/>
-    <sheet name="Sheet1" r:id="rId13" sheetId="2"/>
+    <sheet name="PayNowCCSCF" r:id="rId2" sheetId="5"/>
+    <sheet name="PayNowCCDCF" r:id="rId3" sheetId="6"/>
+    <sheet name="DCFVerbiage" r:id="rId4" sheetId="8"/>
+    <sheet name="OverUnderPay" r:id="rId5" sheetId="9"/>
+    <sheet name="MissingCC" r:id="rId6" sheetId="4"/>
+    <sheet name="Sheet2" r:id="rId7" sheetId="3"/>
+    <sheet name="NoModifyAmount" r:id="rId8" sheetId="10"/>
+    <sheet name="NoOverPay" r:id="rId9" sheetId="11"/>
+    <sheet name="SCFVerbiage" r:id="rId10" sheetId="7"/>
+    <sheet name="Sheet1" r:id="rId11" sheetId="2"/>
+    <sheet name="NoModifyAmountCC" r:id="rId12" sheetId="12"/>
+    <sheet name="NoModifyBillingAddressCC" r:id="rId13" sheetId="13"/>
+    <sheet name="CCDeferredCC" r:id="rId14" sheetId="14"/>
+    <sheet name="CMCAutopayCC" r:id="rId15" sheetId="15"/>
+    <sheet name="PayNowCreditCardDCF" r:id="rId16" sheetId="16"/>
+    <sheet name="PayNowCreditCardSCF" r:id="rId17" sheetId="17"/>
+    <sheet name="DCFCCVerbiage" r:id="rId18" sheetId="18"/>
+    <sheet name="SCFCCVerbiage" r:id="rId19" sheetId="19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="209">
   <si>
     <t>Notes</t>
   </si>
@@ -626,37 +632,52 @@
     <t>Sat Oct 05 17:09:14 EDT 2024</t>
   </si>
   <si>
+    <t>887</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Fri Jan 03 22:06:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jan 06 14:31:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Tue Dec 17 17:02:38 IST 2024</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>883</t>
+  </si>
+  <si>
     <t>882</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Tue Nov 12 17:10:37 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Nov 12 17:12:28 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Nov 12 17:14:08 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Nov 12 17:15:47 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Nov 12 17:16:30 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Nov 12 17:17:16 IST 2024</t>
-  </si>
-  <si>
-    <t>883</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Tue Nov 12 18:48:34 IST 2024</t>
+    <t>Tue Jan 07 15:19:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 07 15:21:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 07 15:23:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 07 15:24:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 07 15:27:17 IST 2025</t>
+  </si>
+  <si>
+    <t>12/31/2025</t>
+  </si>
+  <si>
+    <t>Tue Jan 07 15:29:56 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -720,7 +741,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
@@ -728,6 +749,9 @@
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -1045,8 +1069,8 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="90" zoomScaleNormal="90">
-      <pane activePane="topRight" state="frozen" topLeftCell="D1" xSplit="3"/>
-      <selection pane="topRight" sqref="A1:XFD1048576"/>
+      <pane activePane="topRight" state="frozen" topLeftCell="K1" xSplit="3"/>
+      <selection activeCell="I1" pane="topRight" sqref="I1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1360,323 +1384,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F5F0A8-DFAA-493B-B07B-97C59CBB0D66}">
-  <dimension ref="A1:AC2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.54296875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.81640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.26953125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.1796875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.453125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.453125" collapsed="true"/>
-    <col min="9" max="17" bestFit="true" customWidth="true" width="7.81640625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="8.81640625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="8.54296875" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="17.26953125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="6.54296875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="8.1796875" collapsed="true"/>
-    <col min="23" max="24" bestFit="true" customWidth="true" width="7.453125" collapsed="true"/>
-    <col min="25" max="26" bestFit="true" customWidth="true" width="6.453125" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="8.1796875" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row customFormat="1" ht="29" r="2" s="1" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="AB2" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{133992E5-F2D4-42EB-B2FB-D66167060930}">
-  <dimension ref="A1:AC2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.54296875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.81640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.26953125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.1796875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.453125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.453125" collapsed="true"/>
-    <col min="9" max="17" bestFit="true" customWidth="true" width="7.81640625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="8.81640625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="8.54296875" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="17.26953125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="6.54296875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="8.1796875" collapsed="true"/>
-    <col min="23" max="24" bestFit="true" customWidth="true" width="7.453125" collapsed="true"/>
-    <col min="25" max="26" bestFit="true" customWidth="true" width="6.453125" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="8.1796875" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row customFormat="1" r="2" s="1" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="AB2" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0998B4B-1379-4C62-AAAC-69FB8C23F4B6}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
@@ -1848,7 +1555,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1CECF72-ED76-4A08-B368-44E780FE04C9}">
   <dimension ref="A1:AY4"/>
   <sheetViews>
@@ -2362,307 +2069,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{592A887A-E7FF-45A4-AA15-F82DEC7746C1}">
-  <dimension ref="A1:O7"/>
-  <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:N1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="15.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" style="1" width="15.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.26953125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="43.81640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="12.453125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.1796875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.453125" collapsed="true"/>
-    <col min="7" max="7" style="1" width="15.7265625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.453125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.81640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="17.7265625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="1" width="23.0" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="14.453125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="1" width="15.81640625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="15" max="16384" style="1" width="15.7265625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B3" t="s">
-        <v>196</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>194</v>
-      </c>
-      <c r="B4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B5" t="s">
-        <v>198</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>136</v>
-      </c>
-      <c r="B6" t="s">
-        <v>199</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B7" t="s">
-        <v>200</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC66D8CD-ACD3-4E9A-AD22-471BFACD018F}">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E9DE92-B397-44B0-AEC9-F8D25811CB54}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2711,31 +2123,33 @@
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row ht="101.5" r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C2" s="2"/>
+        <v>195</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>184</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>130</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>91</v>
+        <v>186</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>123</v>
+      <c r="H2" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>176</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>152</v>
@@ -2743,12 +2157,14 @@
       <c r="K2" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>174</v>
+      <c r="L2" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2756,12 +2172,711 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5A0641-6BD7-468B-84F0-EE792C70A080}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row ht="29" r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row ht="101.5" r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D73A527-72BD-4591-A2D4-2CEF61283D2F}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row ht="29" r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row ht="29" r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF51F7AD-B3C1-42AF-94A4-9027DD404D74}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row ht="29" r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAAE4061-05C7-45C5-8300-61EB089304F4}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:N1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row ht="29" r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CCF0244-D738-49E7-A19C-75065FE186E2}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:N1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row ht="29" r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24FF721F-C1CF-4DC8-8195-832F8368F224}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:N1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row ht="29" r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4992758E-A1F9-4281-AE93-21063312FF32}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row ht="29" r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE14908-B016-4D5E-AEA7-D54DB9070BC6}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3024,12 +3139,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{822FCC47-1993-44A8-9BE0-581A41644C90}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3291,7 +3406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0550F98D-701F-463B-8524-B8E5F73F2D8E}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
@@ -3461,7 +3576,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30327A80-5D3D-4DEF-87CB-A4BDC28D6002}">
   <dimension ref="A1:AD5"/>
   <sheetViews>
@@ -3682,7 +3797,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19FB57A2-D7E3-4332-BF3A-D9FD91EC8308}">
   <dimension ref="A1:AY2"/>
   <sheetViews>
@@ -3923,7 +4038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6029C9A2-9E58-4FB9-972D-7B9E934718A7}">
   <dimension ref="A1:C26"/>
   <sheetViews>
@@ -4087,4 +4202,321 @@
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F5F0A8-DFAA-493B-B07B-97C59CBB0D66}">
+  <dimension ref="A1:AC2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.54296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.81640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.26953125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.1796875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.453125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.453125" collapsed="true"/>
+    <col min="9" max="17" bestFit="true" customWidth="true" width="7.81640625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="8.81640625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="8.54296875" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="17.26953125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="6.54296875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="8.1796875" collapsed="true"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" width="7.453125" collapsed="true"/>
+    <col min="25" max="26" bestFit="true" customWidth="true" width="6.453125" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="8.1796875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row customFormat="1" r="1" s="1" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row customFormat="1" ht="29" r="2" s="1" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{133992E5-F2D4-42EB-B2FB-D66167060930}">
+  <dimension ref="A1:AC2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.54296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.81640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.26953125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.1796875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.453125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.453125" collapsed="true"/>
+    <col min="9" max="17" bestFit="true" customWidth="true" width="7.81640625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="8.81640625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="8.54296875" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="17.26953125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="6.54296875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="8.1796875" collapsed="true"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" width="7.453125" collapsed="true"/>
+    <col min="25" max="26" bestFit="true" customWidth="true" width="6.453125" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="8.1796875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row customFormat="1" r="1" s="1" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row customFormat="1" r="2" s="1" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added 27 MV test cases and UnCommented Emulator populate code
</commit_message>
<xml_diff>
--- a/KatalonData/IWPBootstrapData/VRelayPaymentsCC.xlsx
+++ b/KatalonData/IWPBootstrapData/VRelayPaymentsCC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T476640\Documents\VPS_Katalon\VPS-Katalon\KatalonData\IWPBootstrapData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{676EBDAF-86A3-4BC1-A302-49CE2A5FE37D}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{9FDFF3D0-FFFA-45B6-85FF-3B964B78228A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="13" firstSheet="13" windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{19E085DA-5ADF-4B16-9D78-B410FD3FCE3D}" yWindow="-110"/>
+    <workbookView activeTab="18" firstSheet="16" windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{19E085DA-5ADF-4B16-9D78-B410FD3FCE3D}" yWindow="-110"/>
   </bookViews>
   <sheets>
     <sheet name="PayNowCC" r:id="rId1" sheetId="1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="211">
   <si>
     <t>Notes</t>
   </si>
@@ -638,9 +638,6 @@
     <t/>
   </si>
   <si>
-    <t>Fri Jan 03 22:06:40 IST 2025</t>
-  </si>
-  <si>
     <t>Mon Jan 06 14:31:44 IST 2025</t>
   </si>
   <si>
@@ -671,9 +668,6 @@
     <t>Tue Jan 07 15:24:54 IST 2025</t>
   </si>
   <si>
-    <t>Tue Jan 07 15:27:17 IST 2025</t>
-  </si>
-  <si>
     <t>12/31/2025</t>
   </si>
   <si>
@@ -681,6 +675,15 @@
   </si>
   <si>
     <t>Tue Jan 07 15:48:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Jan 24 13:45:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Jan 24 13:56:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Jan 24 13:57:24 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -1073,7 +1076,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="90" zoomScaleNormal="90">
       <pane activePane="topRight" state="frozen" topLeftCell="K1" xSplit="3"/>
-      <selection activeCell="I1" pane="topRight" sqref="I1:N1"/>
+      <selection activeCell="C17" pane="topRight" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2131,7 +2134,7 @@
         <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>184</v>
@@ -2234,7 +2237,7 @@
         <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>184</v>
@@ -2282,7 +2285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D73A527-72BD-4591-A2D4-2CEF61283D2F}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
@@ -2337,7 +2340,7 @@
         <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -2365,7 +2368,7 @@
         <v>177</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>176</v>
@@ -2435,17 +2438,17 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" t="s">
         <v>197</v>
-      </c>
-      <c r="B2" t="s">
-        <v>198</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
         <v>130</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>183</v>
@@ -2537,7 +2540,7 @@
         <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -2547,7 +2550,7 @@
         <v>186</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>182</v>
@@ -2636,7 +2639,7 @@
         <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -2646,7 +2649,7 @@
         <v>186</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>182</v>
@@ -2735,7 +2738,7 @@
         <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -2745,7 +2748,7 @@
         <v>186</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>182</v>
@@ -2779,8 +2782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4992758E-A1F9-4281-AE93-21063312FF32}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2834,7 +2837,7 @@
         <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -2844,7 +2847,7 @@
         <v>186</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>182</v>

</xml_diff>

<commit_message>
Updated RAD test data for new changes
</commit_message>
<xml_diff>
--- a/KatalonData/IWPBootstrapData/VRelayPaymentsCC.xlsx
+++ b/KatalonData/IWPBootstrapData/VRelayPaymentsCC.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="211">
   <si>
     <t>Notes</t>
   </si>
@@ -681,6 +681,9 @@
   </si>
   <si>
     <t>Tue Jan 07 15:48:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Jan 31 21:43:10 EST 2025</t>
   </si>
 </sst>
 </file>
@@ -2537,7 +2540,7 @@
         <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">

</xml_diff>

<commit_message>
Replaced emulatorIWP30,Updated VrelayPamentsCC data
</commit_message>
<xml_diff>
--- a/KatalonData/IWPBootstrapData/VRelayPaymentsCC.xlsx
+++ b/KatalonData/IWPBootstrapData/VRelayPaymentsCC.xlsx
@@ -1,41 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T476640\Documents\VPS_Katalon\VPS-Katalon\KatalonData\IWPBootstrapData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{9FDFF3D0-FFFA-45B6-85FF-3B964B78228A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5131C2DD-03F9-4D8E-BEB8-6E5B4989C323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="18" firstSheet="16" windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{19E085DA-5ADF-4B16-9D78-B410FD3FCE3D}" yWindow="-110"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{19E085DA-5ADF-4B16-9D78-B410FD3FCE3D}"/>
   </bookViews>
   <sheets>
-    <sheet name="PayNowCC" r:id="rId1" sheetId="1"/>
-    <sheet name="PayNowCCSCF" r:id="rId2" sheetId="5"/>
-    <sheet name="PayNowCCDCF" r:id="rId3" sheetId="6"/>
-    <sheet name="DCFVerbiage" r:id="rId4" sheetId="8"/>
-    <sheet name="OverUnderPay" r:id="rId5" sheetId="9"/>
-    <sheet name="MissingCC" r:id="rId6" sheetId="4"/>
-    <sheet name="Sheet2" r:id="rId7" sheetId="3"/>
-    <sheet name="NoModifyAmount" r:id="rId8" sheetId="10"/>
-    <sheet name="NoOverPay" r:id="rId9" sheetId="11"/>
-    <sheet name="SCFVerbiage" r:id="rId10" sheetId="7"/>
-    <sheet name="Sheet1" r:id="rId11" sheetId="2"/>
-    <sheet name="NoModifyAmountCC" r:id="rId12" sheetId="12"/>
-    <sheet name="NoModifyBillingAddressCC" r:id="rId13" sheetId="13"/>
-    <sheet name="CCDeferredCC" r:id="rId14" sheetId="14"/>
-    <sheet name="CMCAutopayCC" r:id="rId15" sheetId="15"/>
-    <sheet name="PayNowCreditCardDCF" r:id="rId16" sheetId="16"/>
-    <sheet name="PayNowCreditCardSCF" r:id="rId17" sheetId="17"/>
-    <sheet name="DCFCCVerbiage" r:id="rId18" sheetId="18"/>
-    <sheet name="SCFCCVerbiage" r:id="rId19" sheetId="19"/>
+    <sheet name="PayNowCC" sheetId="1" r:id="rId1"/>
+    <sheet name="PayNowCCSCF" sheetId="5" r:id="rId2"/>
+    <sheet name="PayNowCCDCF" sheetId="6" r:id="rId3"/>
+    <sheet name="DCFVerbiage" sheetId="8" r:id="rId4"/>
+    <sheet name="OverUnderPay" sheetId="9" r:id="rId5"/>
+    <sheet name="MissingCC" sheetId="4" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId7"/>
+    <sheet name="NoModifyAmount" sheetId="10" r:id="rId8"/>
+    <sheet name="NoOverPay" sheetId="11" r:id="rId9"/>
+    <sheet name="SCFVerbiage" sheetId="7" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId11"/>
+    <sheet name="NoModifyAmountCC" sheetId="12" r:id="rId12"/>
+    <sheet name="NoModifyBillingAddressCC" sheetId="13" r:id="rId13"/>
+    <sheet name="CCDeferredCC" sheetId="14" r:id="rId14"/>
+    <sheet name="CMCAutopayCC" sheetId="15" r:id="rId15"/>
+    <sheet name="PayNowCreditCardDCF" sheetId="16" r:id="rId16"/>
+    <sheet name="PayNowCreditCardSCF" sheetId="17" r:id="rId17"/>
+    <sheet name="DCFCCVerbiage" sheetId="18" r:id="rId18"/>
+    <sheet name="SCFCCVerbiage" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="208">
   <si>
     <t>Notes</t>
   </si>
@@ -638,9 +638,6 @@
     <t/>
   </si>
   <si>
-    <t>Mon Jan 06 14:31:44 IST 2025</t>
-  </si>
-  <si>
     <t>Fail</t>
   </si>
   <si>
@@ -659,15 +656,9 @@
     <t>Tue Jan 07 15:19:24 IST 2025</t>
   </si>
   <si>
-    <t>Tue Jan 07 15:21:09 IST 2025</t>
-  </si>
-  <si>
     <t>Tue Jan 07 15:23:05 IST 2025</t>
   </si>
   <si>
-    <t>Tue Jan 07 15:24:54 IST 2025</t>
-  </si>
-  <si>
     <t>12/31/2025</t>
   </si>
   <si>
@@ -677,16 +668,7 @@
     <t>Tue Jan 07 15:48:01 IST 2025</t>
   </si>
   <si>
-    <t>Fri Jan 24 13:45:18 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Jan 24 13:56:35 IST 2025</t>
-  </si>
-  <si>
     <t>Fri Jan 24 13:57:24 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 05 18:18:42 IST 2025</t>
   </si>
   <si>
     <t>Wed Feb 05 18:20:14 IST 2025</t>
@@ -699,7 +681,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -754,25 +735,25 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -789,10 +770,10 @@
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -827,7 +808,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -879,7 +860,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -990,21 +971,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1021,7 +1002,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1073,38 +1054,38 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office 2013 - 2022 Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4684B99E-74C7-4C50-809D-02154653C064}">
-  <dimension ref="A1:O7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4684B99E-74C7-4C50-809D-02154653C064}">
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="90" zoomScaleNormal="90">
-      <pane activePane="topRight" state="frozen" topLeftCell="K1" xSplit="3"/>
-      <selection activeCell="C17" pane="topRight" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="1" width="15.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.26953125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="43.81640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="12.453125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.1796875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.453125" collapsed="true"/>
-    <col min="7" max="7" style="1" width="15.7265625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.453125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.81640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="17.7265625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="1" width="23.0" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="14.453125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="1" width="15.81640625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="15" max="16384" style="1" width="15.7265625" collapsed="true"/>
+    <col min="1" max="1" width="15.7265625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="43.81640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.453125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.7265625" style="1" collapsed="1"/>
+    <col min="8" max="8" width="10.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="7.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.7265625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23" style="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.453125" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.81640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="16384" width="15.7265625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
@@ -1151,7 +1132,7 @@
         <v>179</v>
       </c>
     </row>
-    <row ht="29" r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>136</v>
       </c>
@@ -1189,7 +1170,7 @@
         <v>177</v>
       </c>
     </row>
-    <row ht="29" r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>136</v>
       </c>
@@ -1227,7 +1208,7 @@
         <v>177</v>
       </c>
     </row>
-    <row ht="29" r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>136</v>
       </c>
@@ -1390,8 +1371,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1399,8 +1380,8 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0998B4B-1379-4C62-AAAC-69FB8C23F4B6}">
-  <dimension ref="A1:AC5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0998B4B-1379-4C62-AAAC-69FB8C23F4B6}">
+  <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="T2" sqref="T2"/>
@@ -1408,29 +1389,29 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="1" width="15.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.26953125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="19.26953125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.1796875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.453125" collapsed="true"/>
-    <col min="7" max="7" style="1" width="15.7265625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.453125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.81640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="15.1796875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="9.7265625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="13.26953125" collapsed="true"/>
-    <col min="13" max="17" bestFit="true" customWidth="true" style="1" width="7.81640625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="8.81640625" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="1" width="17.7265625" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="1" width="23.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.1796875" collapsed="true"/>
-    <col min="23" max="24" bestFit="true" customWidth="true" style="1" width="7.453125" collapsed="true"/>
-    <col min="25" max="26" bestFit="true" customWidth="true" style="1" width="9.1796875" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="29" max="16384" style="1" width="15.7265625" collapsed="true"/>
+    <col min="1" max="1" width="15.7265625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.7265625" style="1" collapsed="1"/>
+    <col min="8" max="8" width="10.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="7.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.1796875" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.26953125" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="17" width="7.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="8.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="17.7265625" style="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="23" style="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.54296875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="24" width="7.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="26" width="9.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="16384" width="15.7265625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.35">
@@ -1566,13 +1547,13 @@
       <c r="B5"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1CECF72-ED76-4A08-B368-44E780FE04C9}">
-  <dimension ref="A1:AY4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1CECF72-ED76-4A08-B368-44E780FE04C9}">
+  <dimension ref="A1:AX4"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="Q42" sqref="Q42"/>
@@ -1580,44 +1561,44 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="38.54296875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="4.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="8.1796875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="8.26953125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="6.81640625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="13.81640625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="9.453125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="5.54296875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="6.1796875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="14.7265625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="23.81640625" collapsed="true"/>
-    <col min="18" max="23" bestFit="true" customWidth="true" style="1" width="9.7265625" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" style="1" width="9.81640625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="6.81640625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="9.7265625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="10.7265625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="6.453125" collapsed="true"/>
-    <col min="29" max="29" style="1" width="15.7265625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="10.453125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="7.81640625" collapsed="true"/>
-    <col min="32" max="33" bestFit="true" customWidth="true" style="1" width="9.7265625" collapsed="true"/>
-    <col min="34" max="39" bestFit="true" customWidth="true" style="1" width="7.81640625" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" style="1" width="8.81640625" collapsed="true"/>
-    <col min="41" max="41" customWidth="true" style="1" width="17.7265625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" style="1" width="17.26953125" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" style="1" width="8.1796875" collapsed="true"/>
-    <col min="45" max="46" bestFit="true" customWidth="true" style="1" width="7.453125" collapsed="true"/>
-    <col min="47" max="48" bestFit="true" customWidth="true" style="1" width="9.1796875" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="51" max="16384" style="1" width="15.7265625" collapsed="true"/>
+    <col min="1" max="1" width="38.54296875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="4" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.54296875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="6.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="5.54296875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="6.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="23.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="23" width="9.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9.81640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="6.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="9.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="10.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="6.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="15.7265625" style="1" collapsed="1"/>
+    <col min="30" max="30" width="10.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="7.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="33" width="9.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="39" width="7.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="8.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="17.7265625" style="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="17.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="6.54296875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="8.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="46" width="7.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="9.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="16384" width="15.7265625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.35">
@@ -2077,7 +2058,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -2085,8 +2066,8 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E9DE92-B397-44B0-AEC9-F8D25811CB54}">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E9DE92-B397-44B0-AEC9-F8D25811CB54}">
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:N2"/>
@@ -2094,7 +2075,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row ht="29" r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -2138,12 +2119,12 @@
         <v>179</v>
       </c>
     </row>
-    <row ht="101.5" r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>184</v>
@@ -2183,13 +2164,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5A0641-6BD7-468B-84F0-EE792C70A080}">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5A0641-6BD7-468B-84F0-EE792C70A080}">
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
@@ -2197,7 +2178,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row ht="29" r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -2241,12 +2222,12 @@
         <v>179</v>
       </c>
     </row>
-    <row ht="101.5" r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>184</v>
@@ -2286,13 +2267,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D73A527-72BD-4591-A2D4-2CEF61283D2F}">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D73A527-72BD-4591-A2D4-2CEF61283D2F}">
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N8" sqref="N8"/>
@@ -2300,7 +2281,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row ht="29" r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -2344,12 +2325,12 @@
         <v>179</v>
       </c>
     </row>
-    <row ht="29" r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -2377,7 +2358,7 @@
         <v>177</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>176</v>
@@ -2387,13 +2368,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF51F7AD-B3C1-42AF-94A4-9027DD404D74}">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF51F7AD-B3C1-42AF-94A4-9027DD404D74}">
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
@@ -2401,7 +2382,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row ht="29" r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -2447,17 +2428,17 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" t="s">
         <v>196</v>
-      </c>
-      <c r="B2" t="s">
-        <v>197</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
         <v>130</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>183</v>
@@ -2486,13 +2467,112 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAAE4061-05C7-45C5-8300-61EB089304F4}">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAAE4061-05C7-45C5-8300-61EB089304F4}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CCF0244-D738-49E7-A19C-75065FE186E2}">
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:N1"/>
@@ -2500,7 +2580,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row ht="29" r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -2549,7 +2629,7 @@
         <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -2585,13 +2665,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CCF0244-D738-49E7-A19C-75065FE186E2}">
-  <dimension ref="A1:O2"/>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24FF721F-C1CF-4DC8-8195-832F8368F224}">
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:N1"/>
@@ -2599,7 +2679,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row ht="29" r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -2648,7 +2728,7 @@
         <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -2658,7 +2738,7 @@
         <v>186</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>182</v>
@@ -2684,120 +2764,21 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24FF721F-C1CF-4DC8-8195-832F8368F224}">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:N1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row ht="29" r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4992758E-A1F9-4281-AE93-21063312FF32}">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4992758E-A1F9-4281-AE93-21063312FF32}">
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row ht="29" r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -2846,7 +2827,7 @@
         <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -2856,7 +2837,7 @@
         <v>186</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>182</v>
@@ -2882,13 +2863,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE14908-B016-4D5E-AEA7-D54DB9070BC6}">
-  <dimension ref="A1:AC5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE14908-B016-4D5E-AEA7-D54DB9070BC6}">
+  <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
@@ -2896,29 +2877,29 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="1" width="15.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.26953125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="19.26953125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.1796875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.453125" collapsed="true"/>
-    <col min="7" max="7" style="1" width="15.7265625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.453125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.81640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="15.1796875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="9.7265625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="13.26953125" collapsed="true"/>
-    <col min="13" max="17" bestFit="true" customWidth="true" style="1" width="7.81640625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="8.81640625" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="1" width="17.7265625" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="1" width="23.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.1796875" collapsed="true"/>
-    <col min="23" max="24" bestFit="true" customWidth="true" style="1" width="7.453125" collapsed="true"/>
-    <col min="25" max="26" bestFit="true" customWidth="true" style="1" width="9.1796875" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="29" max="16384" style="1" width="15.7265625" collapsed="true"/>
+    <col min="1" max="1" width="15.7265625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.7265625" style="1" collapsed="1"/>
+    <col min="8" max="8" width="10.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="7.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.1796875" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.26953125" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="17" width="7.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="8.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="17.7265625" style="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="23" style="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.54296875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="24" width="7.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="26" width="9.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="16384" width="15.7265625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.35">
@@ -3150,13 +3131,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{822FCC47-1993-44A8-9BE0-581A41644C90}">
-  <dimension ref="A1:AC5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{822FCC47-1993-44A8-9BE0-581A41644C90}">
+  <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
@@ -3164,29 +3145,29 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="1" width="15.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.26953125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="19.26953125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.1796875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.453125" collapsed="true"/>
-    <col min="7" max="7" style="1" width="15.7265625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.453125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.81640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="15.1796875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="9.7265625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="13.26953125" collapsed="true"/>
-    <col min="13" max="17" bestFit="true" customWidth="true" style="1" width="7.81640625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="8.81640625" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="1" width="17.7265625" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="1" width="23.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.1796875" collapsed="true"/>
-    <col min="23" max="24" bestFit="true" customWidth="true" style="1" width="7.453125" collapsed="true"/>
-    <col min="25" max="26" bestFit="true" customWidth="true" style="1" width="9.1796875" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="29" max="16384" style="1" width="15.7265625" collapsed="true"/>
+    <col min="1" max="1" width="15.7265625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.7265625" style="1" collapsed="1"/>
+    <col min="8" max="8" width="10.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="7.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.1796875" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.26953125" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="17" width="7.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="8.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="17.7265625" style="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="23" style="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.54296875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="24" width="7.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="26" width="9.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="16384" width="15.7265625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.35">
@@ -3417,13 +3398,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0550F98D-701F-463B-8524-B8E5F73F2D8E}">
-  <dimension ref="A1:AC5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0550F98D-701F-463B-8524-B8E5F73F2D8E}">
+  <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
@@ -3431,29 +3412,29 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="1" width="15.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.26953125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="19.26953125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.1796875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.453125" collapsed="true"/>
-    <col min="7" max="7" style="1" width="15.7265625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.453125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.81640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="15.1796875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="9.7265625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="13.26953125" collapsed="true"/>
-    <col min="13" max="17" bestFit="true" customWidth="true" style="1" width="7.81640625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="8.81640625" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="1" width="17.7265625" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="1" width="23.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.1796875" collapsed="true"/>
-    <col min="23" max="24" bestFit="true" customWidth="true" style="1" width="7.453125" collapsed="true"/>
-    <col min="25" max="26" bestFit="true" customWidth="true" style="1" width="9.1796875" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="29" max="16384" style="1" width="15.7265625" collapsed="true"/>
+    <col min="1" max="1" width="15.7265625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.7265625" style="1" collapsed="1"/>
+    <col min="8" max="8" width="10.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="7.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.1796875" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.26953125" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="17" width="7.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="8.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="17.7265625" style="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="23" style="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.54296875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="24" width="7.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="26" width="9.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="16384" width="15.7265625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.35">
@@ -3587,13 +3568,13 @@
       <c r="B5"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30327A80-5D3D-4DEF-87CB-A4BDC28D6002}">
-  <dimension ref="A1:AD5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30327A80-5D3D-4DEF-87CB-A4BDC28D6002}">
+  <dimension ref="A1:AC5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AC3" sqref="AC3"/>
@@ -3601,30 +3582,30 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="1" width="15.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.26953125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="19.26953125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.1796875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.453125" collapsed="true"/>
-    <col min="7" max="7" style="1" width="15.7265625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.453125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.81640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="15.1796875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="9.7265625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="13.26953125" collapsed="true"/>
-    <col min="13" max="17" bestFit="true" customWidth="true" style="1" width="7.81640625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="8.81640625" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="1" width="17.7265625" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="1" width="23.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.1796875" collapsed="true"/>
-    <col min="23" max="24" bestFit="true" customWidth="true" style="1" width="7.453125" collapsed="true"/>
-    <col min="25" max="26" bestFit="true" customWidth="true" style="1" width="9.1796875" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="1" width="28.1796875" collapsed="true"/>
-    <col min="30" max="16384" style="1" width="15.7265625" collapsed="true"/>
+    <col min="1" max="1" width="15.7265625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.7265625" style="1" collapsed="1"/>
+    <col min="8" max="8" width="10.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="7.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.1796875" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.26953125" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="17" width="7.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="8.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="17.7265625" style="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="23" style="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.54296875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="24" width="7.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="26" width="9.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="28.1796875" style="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="16384" width="15.7265625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.35">
@@ -3716,7 +3697,7 @@
         <v>143</v>
       </c>
     </row>
-    <row ht="29" r="2" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:29" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>136</v>
       </c>
@@ -3808,13 +3789,13 @@
       <c r="B5"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19FB57A2-D7E3-4332-BF3A-D9FD91EC8308}">
-  <dimension ref="A1:AY2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19FB57A2-D7E3-4332-BF3A-D9FD91EC8308}">
+  <dimension ref="A1:AX2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AX6" sqref="AX6"/>
@@ -3822,44 +3803,44 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="49.453125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="4.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="8.1796875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="8.26953125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="6.81640625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="13.81640625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="9.453125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="5.54296875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="6.1796875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="14.7265625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="23.81640625" collapsed="true"/>
-    <col min="18" max="23" bestFit="true" customWidth="true" style="1" width="9.7265625" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" style="1" width="9.81640625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="6.81640625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="9.7265625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="10.7265625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="6.453125" collapsed="true"/>
-    <col min="29" max="29" style="1" width="15.7265625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="10.453125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="7.81640625" collapsed="true"/>
-    <col min="32" max="33" bestFit="true" customWidth="true" style="1" width="9.7265625" collapsed="true"/>
-    <col min="34" max="39" bestFit="true" customWidth="true" style="1" width="7.81640625" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" style="1" width="8.81640625" collapsed="true"/>
-    <col min="41" max="41" customWidth="true" style="1" width="17.7265625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" style="1" width="17.26953125" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" style="1" width="8.1796875" collapsed="true"/>
-    <col min="45" max="46" bestFit="true" customWidth="true" style="1" width="7.453125" collapsed="true"/>
-    <col min="47" max="48" bestFit="true" customWidth="true" style="1" width="9.1796875" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="51" max="16384" style="1" width="15.7265625" collapsed="true"/>
+    <col min="1" max="1" width="49.453125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="4" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.54296875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="6.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="5.54296875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="6.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="23.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="23" width="9.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9.81640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="6.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="9.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="10.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="6.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="15.7265625" style="1" collapsed="1"/>
+    <col min="30" max="30" width="10.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="7.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="33" width="9.7265625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="39" width="7.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="8.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="17.7265625" style="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="17.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="6.54296875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="8.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="46" width="7.453125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="9.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="16384" width="15.7265625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.35">
@@ -4046,7 +4027,7 @@
       <c r="AX2" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -4054,8 +4035,8 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6029C9A2-9E58-4FB9-972D-7B9E934718A7}">
-  <dimension ref="A1:C26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6029C9A2-9E58-4FB9-972D-7B9E934718A7}">
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -4063,7 +4044,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="56.453125" collapsed="true"/>
+    <col min="1" max="1" width="56.453125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -4212,7 +4193,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -4220,8 +4201,8 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F5F0A8-DFAA-493B-B07B-97C59CBB0D66}">
-  <dimension ref="A1:AC2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F5F0A8-DFAA-493B-B07B-97C59CBB0D66}">
+  <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
@@ -4229,27 +4210,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.54296875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.81640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.26953125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.1796875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.453125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.453125" collapsed="true"/>
-    <col min="9" max="17" bestFit="true" customWidth="true" width="7.81640625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="8.81640625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="8.54296875" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="17.26953125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="6.54296875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="8.1796875" collapsed="true"/>
-    <col min="23" max="24" bestFit="true" customWidth="true" width="7.453125" collapsed="true"/>
-    <col min="25" max="26" bestFit="true" customWidth="true" width="6.453125" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="8.1796875" collapsed="true"/>
+    <col min="1" max="1" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="17" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="8.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="17.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="24" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="26" width="6.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -4335,7 +4316,7 @@
         <v>80</v>
       </c>
     </row>
-    <row customFormat="1" ht="29" r="2" s="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>136</v>
       </c>
@@ -4372,13 +4353,13 @@
       <c r="AB2" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{133992E5-F2D4-42EB-B2FB-D66167060930}">
-  <dimension ref="A1:AC2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{133992E5-F2D4-42EB-B2FB-D66167060930}">
+  <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
@@ -4386,27 +4367,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.54296875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.81640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.26953125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.1796875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.453125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.453125" collapsed="true"/>
-    <col min="9" max="17" bestFit="true" customWidth="true" width="7.81640625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="8.81640625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="8.54296875" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="17.26953125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="6.54296875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="8.1796875" collapsed="true"/>
-    <col min="23" max="24" bestFit="true" customWidth="true" width="7.453125" collapsed="true"/>
-    <col min="25" max="26" bestFit="true" customWidth="true" width="6.453125" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="8.1796875" collapsed="true"/>
+    <col min="1" max="1" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="17" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="8.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="17.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="24" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="26" width="6.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -4492,7 +4473,7 @@
         <v>80</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>136</v>
       </c>
@@ -4532,6 +4513,6 @@
       <c r="AB2" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>